<commit_message>
Revise description of data and screening value sources; Correct some spelling errors.
</commit_message>
<xml_diff>
--- a/Derived_Data/Marine_Sediment_Screening_Values.xlsx
+++ b/Derived_Data/Marine_Sediment_Screening_Values.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbohl\Dropbox\Work\Portland Dredge Toxicity Data\Original Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\curtis.bohlen\Documents\State of the Bay 2020\Data\B15. Toxics\PortlandHarborToxics\Derived_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE1808F-91D6-49E5-AB51-C204BF60B68B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="270" windowWidth="16920" windowHeight="10990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1800" yWindow="276" windowWidth="16920" windowHeight="10992"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
     <sheet name="Pesticides" sheetId="6" r:id="rId5"/>
     <sheet name="PCB Nomenclature" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1762,13 +1761,13 @@
     <t xml:space="preserve">https://response.restoration.noaa.gov/environmental-restoration/environmental-assessment-tools/squirt-cards-faq.html </t>
   </si>
   <si>
-    <t>All data from squirts wer typed in by hand, by Curtis C. Bohlen, Sept. 17, 2019.</t>
+    <t>All data from squirts were typed in by hand, by Curtis C. Bohlen, Sept. 17, 2019.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2248,100 +2247,100 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:A22"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>573</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>574</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="A17" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="A20" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A9" r:id="rId1"/>
+    <hyperlink ref="A17" r:id="rId2"/>
+    <hyperlink ref="A20" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId4"/>
@@ -2349,21 +2348,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="55.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.7265625" customWidth="1"/>
-    <col min="4" max="11" width="15.7265625" customWidth="1"/>
+    <col min="2" max="2" width="55.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.77734375" customWidth="1"/>
+    <col min="4" max="11" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>21</v>
       </c>
@@ -2392,7 +2391,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -2412,7 +2411,7 @@
       <c r="I2" s="18"/>
       <c r="J2" s="18"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4" s="10" t="s">
         <v>11</v>
       </c>
@@ -2444,7 +2443,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
         <v>13</v>
       </c>
@@ -2476,7 +2475,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6" s="9" t="s">
         <v>14</v>
       </c>
@@ -2508,7 +2507,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7" s="9" t="s">
         <v>15</v>
       </c>
@@ -2540,7 +2539,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" s="9" t="s">
         <v>16</v>
       </c>
@@ -2572,7 +2571,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" s="9" t="s">
         <v>17</v>
       </c>
@@ -2604,7 +2603,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" s="9" t="s">
         <v>18</v>
       </c>
@@ -2636,7 +2635,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11" s="9" t="s">
         <v>23</v>
       </c>
@@ -2666,7 +2665,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -2701,7 +2700,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13" s="9" t="s">
         <v>20</v>
       </c>
@@ -2742,20 +2741,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="15.7265625" customWidth="1"/>
+    <col min="2" max="2" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>21</v>
       </c>
@@ -2784,7 +2783,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -2804,7 +2803,7 @@
       <c r="I2" s="18"/>
       <c r="J2" s="18"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4" s="10" t="s">
         <v>11</v>
       </c>
@@ -2836,7 +2835,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6" s="12" t="s">
         <v>51</v>
       </c>
@@ -2868,7 +2867,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7" s="12" t="s">
         <v>52</v>
       </c>
@@ -2900,7 +2899,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" s="12" t="s">
         <v>53</v>
       </c>
@@ -2932,7 +2931,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" s="12" t="s">
         <v>54</v>
       </c>
@@ -2964,7 +2963,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" s="12" t="s">
         <v>55</v>
       </c>
@@ -2996,7 +2995,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11" s="12" t="s">
         <v>56</v>
       </c>
@@ -3013,7 +3012,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12" s="12" t="s">
         <v>57</v>
       </c>
@@ -3033,7 +3032,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13" s="12" t="s">
         <v>58</v>
       </c>
@@ -3050,7 +3049,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" s="12" t="s">
         <v>59</v>
       </c>
@@ -3082,7 +3081,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15" s="12" t="s">
         <v>60</v>
       </c>
@@ -3114,7 +3113,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16" s="12" t="s">
         <v>61</v>
       </c>
@@ -3146,7 +3145,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B17" s="12" t="s">
         <v>82</v>
       </c>
@@ -3178,7 +3177,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B18" s="12" t="s">
         <v>62</v>
       </c>
@@ -3198,7 +3197,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B19" s="12" t="s">
         <v>63</v>
       </c>
@@ -3230,7 +3229,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B20" s="12" t="s">
         <v>64</v>
       </c>
@@ -3262,7 +3261,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>68</v>
       </c>
@@ -3270,7 +3269,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>65</v>
       </c>
@@ -3278,7 +3277,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>69</v>
       </c>
@@ -3286,7 +3285,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>66</v>
       </c>
@@ -3294,7 +3293,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -3305,7 +3304,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -3316,7 +3315,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -3327,7 +3326,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -3338,7 +3337,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -3349,7 +3348,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -3360,7 +3359,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>24</v>
       </c>
@@ -3371,7 +3370,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -3392,22 +3391,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I3" workbookViewId="0">
+    <sheetView topLeftCell="I37" workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="32.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="15.7265625" customWidth="1"/>
-    <col min="7" max="7" width="25.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="15.7265625" customWidth="1"/>
+    <col min="3" max="3" width="32.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="15.77734375" customWidth="1"/>
+    <col min="7" max="7" width="25.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D1" t="s">
         <v>21</v>
       </c>
@@ -3436,7 +3435,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -3456,7 +3455,7 @@
       <c r="K2" s="18"/>
       <c r="L2" s="18"/>
     </row>
-    <row r="4" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>543</v>
       </c>
@@ -3494,7 +3493,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B6">
         <f>VALUE(MID(D6,FIND("#",D6)+1,30))</f>
         <v>8</v>
@@ -3510,7 +3509,7 @@
         <v>0.20830000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B7">
         <f t="shared" ref="B7:B21" si="0">VALUE(MID(D7,FIND("#",D7)+1,30))</f>
         <v>18</v>
@@ -3523,7 +3522,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B8">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -3536,7 +3535,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -3549,7 +3548,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B10">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -3562,7 +3561,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -3575,7 +3574,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B12">
         <f t="shared" si="0"/>
         <v>66</v>
@@ -3588,7 +3587,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B13">
         <f t="shared" si="0"/>
         <v>87</v>
@@ -3601,7 +3600,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B14">
         <f t="shared" si="0"/>
         <v>101</v>
@@ -3614,7 +3613,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B15">
         <f t="shared" si="0"/>
         <v>105</v>
@@ -3627,7 +3626,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B16">
         <f t="shared" si="0"/>
         <v>118</v>
@@ -3640,7 +3639,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17">
         <f t="shared" si="0"/>
         <v>128</v>
@@ -3653,7 +3652,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18">
         <f t="shared" si="0"/>
         <v>138</v>
@@ -3666,7 +3665,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19">
         <f t="shared" si="0"/>
         <v>153</v>
@@ -3679,7 +3678,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20">
         <f t="shared" si="0"/>
         <v>170</v>
@@ -3692,7 +3691,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21">
         <f t="shared" si="0"/>
         <v>180</v>
@@ -3705,7 +3704,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
         <v>70</v>
       </c>
@@ -3743,21 +3742,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" customWidth="1"/>
-    <col min="2" max="2" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="11" width="15.7265625" customWidth="1"/>
+    <col min="1" max="1" width="15.77734375" customWidth="1"/>
+    <col min="2" max="2" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>21</v>
       </c>
@@ -3786,7 +3785,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>22</v>
       </c>
@@ -3803,7 +3802,7 @@
       <c r="I2" s="18"/>
       <c r="J2" s="18"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4" s="10" t="s">
         <v>11</v>
       </c>
@@ -3835,7 +3834,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5" s="12" t="s">
         <v>544</v>
       </c>
@@ -3858,7 +3857,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6" s="12" t="s">
         <v>545</v>
       </c>
@@ -3881,7 +3880,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7" s="12" t="s">
         <v>546</v>
       </c>
@@ -3904,7 +3903,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" s="12" t="s">
         <v>547</v>
       </c>
@@ -3915,7 +3914,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>564</v>
       </c>
@@ -3923,12 +3922,12 @@
         <v>548</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" s="12" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11" s="12" t="s">
         <v>565</v>
       </c>
@@ -3957,7 +3956,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>567</v>
       </c>
@@ -3965,17 +3964,17 @@
         <v>550</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13" s="12" t="s">
         <v>551</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" s="12" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15" s="12" t="s">
         <v>553</v>
       </c>
@@ -3992,7 +3991,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16" s="12" t="s">
         <v>554</v>
       </c>
@@ -4003,7 +4002,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>570</v>
       </c>
@@ -4017,7 +4016,7 @@
         <v>2.74</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B18" s="12" t="s">
         <v>555</v>
       </c>
@@ -4028,17 +4027,17 @@
         <v>571</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B19" s="12" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B20" s="12" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B22" s="12" t="s">
         <v>562</v>
       </c>
@@ -4070,23 +4069,23 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E211"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="13.81640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.81640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.1796875" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" style="14"/>
+    <col min="1" max="1" width="17.77734375" style="14" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.21875" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>83</v>
       </c>
@@ -4103,7 +4102,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="15" t="s">
         <v>87</v>
       </c>
@@ -4114,7 +4113,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>89</v>
       </c>
@@ -4131,7 +4130,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>92</v>
       </c>
@@ -4148,7 +4147,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>92</v>
       </c>
@@ -4165,7 +4164,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>97</v>
       </c>
@@ -4182,7 +4181,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>89</v>
       </c>
@@ -4199,7 +4198,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>89</v>
       </c>
@@ -4216,7 +4215,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
         <v>89</v>
       </c>
@@ -4233,7 +4232,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
         <v>89</v>
       </c>
@@ -4250,7 +4249,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
         <v>89</v>
       </c>
@@ -4267,7 +4266,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
         <v>97</v>
       </c>
@@ -4284,7 +4283,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
         <v>112</v>
       </c>
@@ -4301,7 +4300,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>92</v>
       </c>
@@ -4318,7 +4317,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
         <v>92</v>
       </c>
@@ -4335,7 +4334,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
         <v>112</v>
       </c>
@@ -4352,7 +4351,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
         <v>121</v>
       </c>
@@ -4369,7 +4368,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16" t="s">
         <v>97</v>
       </c>
@@ -4386,7 +4385,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="16" t="s">
         <v>97</v>
       </c>
@@ -4403,7 +4402,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
         <v>97</v>
       </c>
@@ -4420,7 +4419,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
         <v>97</v>
       </c>
@@ -4437,7 +4436,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
         <v>132</v>
       </c>
@@ -4454,7 +4453,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
         <v>89</v>
       </c>
@@ -4471,7 +4470,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16" t="s">
         <v>89</v>
       </c>
@@ -4488,7 +4487,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="16" t="s">
         <v>132</v>
       </c>
@@ -4505,7 +4504,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="16" t="s">
         <v>97</v>
       </c>
@@ -4522,7 +4521,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="16" t="s">
         <v>89</v>
       </c>
@@ -4539,7 +4538,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16" t="s">
         <v>132</v>
       </c>
@@ -4556,7 +4555,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="16" t="s">
         <v>97</v>
       </c>
@@ -4573,7 +4572,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="16" t="s">
         <v>149</v>
       </c>
@@ -4590,7 +4589,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="16" t="s">
         <v>89</v>
       </c>
@@ -4607,7 +4606,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="16" t="s">
         <v>97</v>
       </c>
@@ -4624,7 +4623,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="16" t="s">
         <v>89</v>
       </c>
@@ -4641,7 +4640,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16" t="s">
         <v>97</v>
       </c>
@@ -4658,7 +4657,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="16" t="s">
         <v>89</v>
       </c>
@@ -4675,7 +4674,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="16" t="s">
         <v>132</v>
       </c>
@@ -4692,7 +4691,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="16" t="s">
         <v>112</v>
       </c>
@@ -4709,7 +4708,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="16" t="s">
         <v>112</v>
       </c>
@@ -4726,7 +4725,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="16" t="s">
         <v>121</v>
       </c>
@@ -4743,7 +4742,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="16" t="s">
         <v>112</v>
       </c>
@@ -4760,7 +4759,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="16" t="s">
         <v>112</v>
       </c>
@@ -4777,7 +4776,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="16" t="s">
         <v>174</v>
       </c>
@@ -4794,7 +4793,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="16" t="s">
         <v>177</v>
       </c>
@@ -4811,7 +4810,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="16" t="s">
         <v>177</v>
       </c>
@@ -4828,7 +4827,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="16" t="s">
         <v>174</v>
       </c>
@@ -4845,7 +4844,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="16" t="s">
         <v>174</v>
       </c>
@@ -4862,7 +4861,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="16" t="s">
         <v>177</v>
       </c>
@@ -4879,7 +4878,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="16" t="s">
         <v>177</v>
       </c>
@@ -4896,7 +4895,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="16" t="s">
         <v>190</v>
       </c>
@@ -4913,7 +4912,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="16" t="s">
         <v>177</v>
       </c>
@@ -4930,7 +4929,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="16" t="s">
         <v>177</v>
       </c>
@@ -4947,7 +4946,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="16" t="s">
         <v>177</v>
       </c>
@@ -4964,7 +4963,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="16" t="s">
         <v>177</v>
       </c>
@@ -4981,7 +4980,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="16" t="s">
         <v>174</v>
       </c>
@@ -4998,7 +4997,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="16" t="s">
         <v>177</v>
       </c>
@@ -5015,7 +5014,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="16" t="s">
         <v>177</v>
       </c>
@@ -5032,7 +5031,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="16" t="s">
         <v>207</v>
       </c>
@@ -5049,7 +5048,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="16" t="s">
         <v>207</v>
       </c>
@@ -5066,7 +5065,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="16" t="s">
         <v>207</v>
       </c>
@@ -5083,7 +5082,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="16" t="s">
         <v>207</v>
       </c>
@@ -5100,7 +5099,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="16" t="s">
         <v>174</v>
       </c>
@@ -5117,7 +5116,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="16" t="s">
         <v>218</v>
       </c>
@@ -5134,7 +5133,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="16" t="s">
         <v>207</v>
       </c>
@@ -5151,7 +5150,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="16" t="s">
         <v>177</v>
       </c>
@@ -5168,7 +5167,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="16" t="s">
         <v>207</v>
       </c>
@@ -5185,7 +5184,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="16" t="s">
         <v>177</v>
       </c>
@@ -5202,7 +5201,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="16" t="s">
         <v>174</v>
       </c>
@@ -5219,7 +5218,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="16" t="s">
         <v>218</v>
       </c>
@@ -5236,7 +5235,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="16" t="s">
         <v>207</v>
       </c>
@@ -5253,7 +5252,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="16" t="s">
         <v>207</v>
       </c>
@@ -5270,7 +5269,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="16" t="s">
         <v>177</v>
       </c>
@@ -5287,7 +5286,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="16" t="s">
         <v>207</v>
       </c>
@@ -5304,7 +5303,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="16" t="s">
         <v>177</v>
       </c>
@@ -5321,7 +5320,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="16" t="s">
         <v>207</v>
       </c>
@@ -5338,7 +5337,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="16" t="s">
         <v>174</v>
       </c>
@@ -5355,7 +5354,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="16" t="s">
         <v>218</v>
       </c>
@@ -5372,7 +5371,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="16" t="s">
         <v>190</v>
       </c>
@@ -5389,7 +5388,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="16" t="s">
         <v>207</v>
       </c>
@@ -5406,7 +5405,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="16" t="s">
         <v>253</v>
       </c>
@@ -5423,7 +5422,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="16" t="s">
         <v>256</v>
       </c>
@@ -5440,7 +5439,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="16" t="s">
         <v>256</v>
       </c>
@@ -5457,7 +5456,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="16" t="s">
         <v>256</v>
       </c>
@@ -5474,7 +5473,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="16" t="s">
         <v>253</v>
       </c>
@@ -5491,7 +5490,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="16" t="s">
         <v>174</v>
       </c>
@@ -5508,7 +5507,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="16" t="s">
         <v>174</v>
       </c>
@@ -5525,7 +5524,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="16" t="s">
         <v>174</v>
       </c>
@@ -5542,7 +5541,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="16" t="s">
         <v>190</v>
       </c>
@@ -5559,7 +5558,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="16" t="s">
         <v>174</v>
       </c>
@@ -5576,7 +5575,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="16" t="s">
         <v>174</v>
       </c>
@@ -5593,7 +5592,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="16" t="s">
         <v>177</v>
       </c>
@@ -5610,7 +5609,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="16" t="s">
         <v>177</v>
       </c>
@@ -5627,7 +5626,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="16" t="s">
         <v>174</v>
       </c>
@@ -5644,7 +5643,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="16" t="s">
         <v>177</v>
       </c>
@@ -5661,7 +5660,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="16" t="s">
         <v>174</v>
       </c>
@@ -5678,7 +5677,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="16" t="s">
         <v>174</v>
       </c>
@@ -5695,7 +5694,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="16" t="s">
         <v>174</v>
       </c>
@@ -5712,7 +5711,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="16" t="s">
         <v>174</v>
       </c>
@@ -5729,7 +5728,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="16" t="s">
         <v>177</v>
       </c>
@@ -5746,7 +5745,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="16" t="s">
         <v>174</v>
       </c>
@@ -5763,7 +5762,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="16" t="s">
         <v>177</v>
       </c>
@@ -5780,7 +5779,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="16" t="s">
         <v>190</v>
       </c>
@@ -5797,7 +5796,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="16" t="s">
         <v>190</v>
       </c>
@@ -5814,7 +5813,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="16" t="s">
         <v>174</v>
       </c>
@@ -5831,7 +5830,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="16" t="s">
         <v>177</v>
       </c>
@@ -5848,7 +5847,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="16" t="s">
         <v>177</v>
       </c>
@@ -5865,7 +5864,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="16" t="s">
         <v>177</v>
       </c>
@@ -5882,7 +5881,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="16" t="s">
         <v>311</v>
       </c>
@@ -5899,7 +5898,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="16" t="s">
         <v>207</v>
       </c>
@@ -5916,7 +5915,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="16" t="s">
         <v>207</v>
       </c>
@@ -5933,7 +5932,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="16" t="s">
         <v>207</v>
       </c>
@@ -5950,7 +5949,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="16" t="s">
         <v>174</v>
       </c>
@@ -5967,7 +5966,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="16" t="s">
         <v>174</v>
       </c>
@@ -5984,7 +5983,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="16" t="s">
         <v>207</v>
       </c>
@@ -6001,7 +6000,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="16" t="s">
         <v>174</v>
       </c>
@@ -6018,7 +6017,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="16" t="s">
         <v>174</v>
       </c>
@@ -6035,7 +6034,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="16" t="s">
         <v>311</v>
       </c>
@@ -6052,7 +6051,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="16" t="s">
         <v>190</v>
       </c>
@@ -6069,7 +6068,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="16" t="s">
         <v>174</v>
       </c>
@@ -6086,7 +6085,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="16" t="s">
         <v>174</v>
       </c>
@@ -6103,7 +6102,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="16" t="s">
         <v>311</v>
       </c>
@@ -6120,7 +6119,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="16" t="s">
         <v>190</v>
       </c>
@@ -6137,7 +6136,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="16" t="s">
         <v>207</v>
       </c>
@@ -6154,7 +6153,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="16" t="s">
         <v>174</v>
       </c>
@@ -6171,7 +6170,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="16" t="s">
         <v>207</v>
       </c>
@@ -6188,7 +6187,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="16" t="s">
         <v>311</v>
       </c>
@@ -6205,7 +6204,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="126" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="16" t="s">
         <v>207</v>
       </c>
@@ -6222,7 +6221,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="127" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="16" t="s">
         <v>174</v>
       </c>
@@ -6239,7 +6238,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="128" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="16" t="s">
         <v>253</v>
       </c>
@@ -6256,7 +6255,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="16" t="s">
         <v>256</v>
       </c>
@@ -6273,7 +6272,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="16" t="s">
         <v>358</v>
       </c>
@@ -6290,7 +6289,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="16" t="s">
         <v>174</v>
       </c>
@@ -6307,7 +6306,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="16" t="s">
         <v>174</v>
       </c>
@@ -6324,7 +6323,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="16" t="s">
         <v>174</v>
       </c>
@@ -6341,7 +6340,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="16" t="s">
         <v>174</v>
       </c>
@@ -6358,7 +6357,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="16" t="s">
         <v>174</v>
       </c>
@@ -6375,7 +6374,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="16" t="s">
         <v>174</v>
       </c>
@@ -6392,7 +6391,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="16" t="s">
         <v>174</v>
       </c>
@@ -6409,7 +6408,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="16" t="s">
         <v>174</v>
       </c>
@@ -6426,7 +6425,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="139" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="16" t="s">
         <v>358</v>
       </c>
@@ -6443,7 +6442,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="16" t="s">
         <v>358</v>
       </c>
@@ -6460,7 +6459,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="16" t="s">
         <v>190</v>
       </c>
@@ -6477,7 +6476,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="142" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="16" t="s">
         <v>190</v>
       </c>
@@ -6494,7 +6493,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="16" t="s">
         <v>174</v>
       </c>
@@ -6511,7 +6510,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="16" t="s">
         <v>174</v>
       </c>
@@ -6528,7 +6527,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="145" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="16" t="s">
         <v>174</v>
       </c>
@@ -6545,7 +6544,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="146" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="16" t="s">
         <v>174</v>
       </c>
@@ -6562,7 +6561,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="147" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="16" t="s">
         <v>177</v>
       </c>
@@ -6579,7 +6578,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="148" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="16" t="s">
         <v>174</v>
       </c>
@@ -6596,7 +6595,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="149" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="16" t="s">
         <v>174</v>
       </c>
@@ -6613,7 +6612,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="150" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="16" t="s">
         <v>174</v>
       </c>
@@ -6630,7 +6629,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="151" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="16" t="s">
         <v>174</v>
       </c>
@@ -6647,7 +6646,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="152" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="16" t="s">
         <v>177</v>
       </c>
@@ -6664,7 +6663,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="153" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="16" t="s">
         <v>174</v>
       </c>
@@ -6681,7 +6680,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="154" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="16" t="s">
         <v>174</v>
       </c>
@@ -6698,7 +6697,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="16" t="s">
         <v>358</v>
       </c>
@@ -6715,7 +6714,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="156" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="16" t="s">
         <v>190</v>
       </c>
@@ -6732,7 +6731,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="157" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="16" t="s">
         <v>190</v>
       </c>
@@ -6749,7 +6748,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="158" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="16" t="s">
         <v>311</v>
       </c>
@@ -6766,7 +6765,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="159" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="16" t="s">
         <v>311</v>
       </c>
@@ -6783,7 +6782,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="160" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="16" t="s">
         <v>358</v>
       </c>
@@ -6800,7 +6799,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="161" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="16" t="s">
         <v>207</v>
       </c>
@@ -6817,7 +6816,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="162" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="16" t="s">
         <v>174</v>
       </c>
@@ -6834,7 +6833,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="163" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="16" t="s">
         <v>174</v>
       </c>
@@ -6851,7 +6850,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="164" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="16" t="s">
         <v>207</v>
       </c>
@@ -6868,7 +6867,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="165" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="16" t="s">
         <v>174</v>
       </c>
@@ -6885,7 +6884,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="166" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="16" t="s">
         <v>174</v>
       </c>
@@ -6902,7 +6901,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="167" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="16" t="s">
         <v>174</v>
       </c>
@@ -6919,7 +6918,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="168" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="16" t="s">
         <v>358</v>
       </c>
@@ -6936,7 +6935,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="169" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="16" t="s">
         <v>311</v>
       </c>
@@ -6953,7 +6952,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="170" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="16" t="s">
         <v>358</v>
       </c>
@@ -6970,7 +6969,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="171" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="16" t="s">
         <v>253</v>
       </c>
@@ -6987,7 +6986,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="172" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="16" t="s">
         <v>358</v>
       </c>
@@ -7004,7 +7003,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="173" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="16" t="s">
         <v>358</v>
       </c>
@@ -7021,7 +7020,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="174" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="16" t="s">
         <v>174</v>
       </c>
@@ -7038,7 +7037,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="175" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="16" t="s">
         <v>174</v>
       </c>
@@ -7055,7 +7054,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="176" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="16" t="s">
         <v>174</v>
       </c>
@@ -7072,7 +7071,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="177" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="16" t="s">
         <v>174</v>
       </c>
@@ -7089,7 +7088,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="178" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="16" t="s">
         <v>174</v>
       </c>
@@ -7106,7 +7105,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="179" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="16" t="s">
         <v>174</v>
       </c>
@@ -7123,7 +7122,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="180" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="16" t="s">
         <v>174</v>
       </c>
@@ -7140,7 +7139,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="181" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="16" t="s">
         <v>174</v>
       </c>
@@ -7157,7 +7156,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="182" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="16" t="s">
         <v>358</v>
       </c>
@@ -7174,7 +7173,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="183" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="16" t="s">
         <v>358</v>
       </c>
@@ -7191,7 +7190,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="184" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" s="16" t="s">
         <v>358</v>
       </c>
@@ -7208,7 +7207,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="185" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="16" t="s">
         <v>358</v>
       </c>
@@ -7225,7 +7224,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="186" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="16" t="s">
         <v>190</v>
       </c>
@@ -7242,7 +7241,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="187" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" s="16" t="s">
         <v>174</v>
       </c>
@@ -7259,7 +7258,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="188" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" s="16" t="s">
         <v>174</v>
       </c>
@@ -7276,7 +7275,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="189" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" s="16" t="s">
         <v>174</v>
       </c>
@@ -7293,7 +7292,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="190" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" s="16" t="s">
         <v>174</v>
       </c>
@@ -7310,7 +7309,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="191" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" s="16" t="s">
         <v>311</v>
       </c>
@@ -7327,7 +7326,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="192" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" s="16" t="s">
         <v>358</v>
       </c>
@@ -7344,7 +7343,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="193" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" s="16" t="s">
         <v>358</v>
       </c>
@@ -7361,7 +7360,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="194" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" s="16" t="s">
         <v>174</v>
       </c>
@@ -7378,7 +7377,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="195" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" s="16" t="s">
         <v>174</v>
       </c>
@@ -7395,7 +7394,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="196" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" s="16" t="s">
         <v>358</v>
       </c>
@@ -7412,7 +7411,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="197" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" s="16" t="s">
         <v>358</v>
       </c>
@@ -7429,7 +7428,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="198" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A198" s="16" t="s">
         <v>358</v>
       </c>
@@ -7446,7 +7445,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="199" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" s="16" t="s">
         <v>358</v>
       </c>
@@ -7463,7 +7462,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="200" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" s="16" t="s">
         <v>174</v>
       </c>
@@ -7480,7 +7479,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="201" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" s="16" t="s">
         <v>174</v>
       </c>
@@ -7497,7 +7496,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="202" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" s="16" t="s">
         <v>174</v>
       </c>
@@ -7514,7 +7513,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="203" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" s="16" t="s">
         <v>174</v>
       </c>
@@ -7531,7 +7530,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="204" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="16" t="s">
         <v>174</v>
       </c>
@@ -7548,7 +7547,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="205" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="16" t="s">
         <v>358</v>
       </c>
@@ -7565,7 +7564,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="206" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="16" t="s">
         <v>358</v>
       </c>
@@ -7582,7 +7581,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="207" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="16" t="s">
         <v>358</v>
       </c>
@@ -7599,7 +7598,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="208" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="16" t="s">
         <v>358</v>
       </c>
@@ -7616,7 +7615,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="209" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" s="16" t="s">
         <v>358</v>
       </c>
@@ -7633,7 +7632,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="210" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A210" s="16" t="s">
         <v>174</v>
       </c>
@@ -7650,7 +7649,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="211" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" s="16" t="s">
         <v>97</v>
       </c>

</xml_diff>